<commit_message>
Strings sync  for products description names between the bridge and the data raw
</commit_message>
<xml_diff>
--- a/data_in/table.correspondences/exio3.to.threeMeEurostat.xlsx
+++ b/data_in/table.correspondences/exio3.to.threeMeEurostat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMalliet\Documents\GitHub\MRIO-Analysis\EXIOBASE\data\table.correspondences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/Professionnel/Github/EmissionsIndicators/data_in/table.correspondences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA2789-E1D7-4054-82CB-5FF1627B81BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB0F217-1817-244B-B2AC-A99DBD9014AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sectors" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="560">
   <si>
     <t>Cultivation of paddy rice</t>
   </si>
@@ -1191,12 +1191,6 @@
     <t>Manure (biogas treatment)</t>
   </si>
   <si>
-    <t>Products of forestry, logging and related services</t>
-  </si>
-  <si>
-    <t>Fish and other fishing products; services incidental of fishing</t>
-  </si>
-  <si>
     <t>Anthracite</t>
   </si>
   <si>
@@ -1231,9 +1225,6 @@
   </si>
   <si>
     <t>Other Hydrocarbons</t>
-  </si>
-  <si>
-    <t>Uranium and thorium ores</t>
   </si>
   <si>
     <t>Iron ores</t>
@@ -1296,21 +1287,6 @@
     <t>Fish products</t>
   </si>
   <si>
-    <t>Tobacco products</t>
-  </si>
-  <si>
-    <t>Textiles</t>
-  </si>
-  <si>
-    <t>Wearing apparel; furs</t>
-  </si>
-  <si>
-    <t>Leather and leather products</t>
-  </si>
-  <si>
-    <t>Wood and products of wood and cork (except furniture); articles of straw and plaiting materials</t>
-  </si>
-  <si>
     <t>Wood material for treatment, Re-processing of secondary wood material into new wood material</t>
   </si>
   <si>
@@ -1318,9 +1294,6 @@
   </si>
   <si>
     <t>Paper and paper products</t>
-  </si>
-  <si>
-    <t>Printed matter and recorded media</t>
   </si>
   <si>
     <t>Coke Oven Coke</t>
@@ -1407,9 +1380,6 @@
     <t>Other Liquid Biofuels</t>
   </si>
   <si>
-    <t>Rubber and plastic products</t>
-  </si>
-  <si>
     <t>Glass and glass products</t>
   </si>
   <si>
@@ -1468,33 +1438,6 @@
   </si>
   <si>
     <t>Foundry work services</t>
-  </si>
-  <si>
-    <t>Fabricated metal products, except machinery and equipment</t>
-  </si>
-  <si>
-    <t>Machinery and equipment n.e.c.</t>
-  </si>
-  <si>
-    <t>Office machinery and computers</t>
-  </si>
-  <si>
-    <t>Electrical machinery and apparatus n.e.c.</t>
-  </si>
-  <si>
-    <t>Radio, television and communication equipment and apparatus</t>
-  </si>
-  <si>
-    <t>Medical, precision and optical instruments, watches and clocks</t>
-  </si>
-  <si>
-    <t>Motor vehicles, trailers and semi-trailers</t>
-  </si>
-  <si>
-    <t>Other transport equipment</t>
-  </si>
-  <si>
-    <t>Furniture; other manufactured goods n.e.c.</t>
   </si>
   <si>
     <t>Secondary raw materials</t>
@@ -1566,25 +1509,10 @@
     <t>Steam and hot water supply services</t>
   </si>
   <si>
-    <t>Collected and purified water, distribution services of water</t>
-  </si>
-  <si>
-    <t>Construction work</t>
-  </si>
-  <si>
     <t>Secondary construction material for treatment, Re-processing of secondary construction material into aggregates</t>
   </si>
   <si>
     <t>Retail trade services of motor fuel</t>
-  </si>
-  <si>
-    <t>Wholesale trade and commission trade services, except of motor vehicles and motorcycles</t>
-  </si>
-  <si>
-    <t>Retail  trade services, except of motor vehicles and motorcycles; repair services of personal and household goods</t>
-  </si>
-  <si>
-    <t>Hotel and restaurant services</t>
   </si>
   <si>
     <t>Railway transportation services</t>
@@ -1600,48 +1528,6 @@
   </si>
   <si>
     <t>Inland water transportation services</t>
-  </si>
-  <si>
-    <t>Air transport services</t>
-  </si>
-  <si>
-    <t>Supporting and auxiliary transport services; travel agency services</t>
-  </si>
-  <si>
-    <t>Post and telecommunication services</t>
-  </si>
-  <si>
-    <t>Financial intermediation services, except insurance and pension funding services</t>
-  </si>
-  <si>
-    <t>Insurance and pension funding services, except compulsory social security services</t>
-  </si>
-  <si>
-    <t>Services auxiliary to financial intermediation</t>
-  </si>
-  <si>
-    <t>Real estate services</t>
-  </si>
-  <si>
-    <t>Renting services of machinery and equipment without operator and of personal and household goods</t>
-  </si>
-  <si>
-    <t>Computer and related services</t>
-  </si>
-  <si>
-    <t>Research and development services</t>
-  </si>
-  <si>
-    <t>Other business services</t>
-  </si>
-  <si>
-    <t>Public administration and defence services; compulsory social security services</t>
-  </si>
-  <si>
-    <t>Education services</t>
-  </si>
-  <si>
-    <t>Health and social work services</t>
   </si>
   <si>
     <t>Food waste for treatment: incineration</t>
@@ -1704,13 +1590,130 @@
     <t>Wood waste for treatment: landfill</t>
   </si>
   <si>
-    <t>Membership organisation services n.e.c.</t>
+    <t>Products of forestry, logging and related services (02)</t>
   </si>
   <si>
-    <t>Recreational, cultural and sporting services</t>
+    <t>Fish and other fishing products; services incidental of fishing (05)</t>
   </si>
   <si>
-    <t>Other services</t>
+    <t>Uranium and thorium ores (12)</t>
+  </si>
+  <si>
+    <t>Tobacco products (16)</t>
+  </si>
+  <si>
+    <t>Textiles (17)</t>
+  </si>
+  <si>
+    <t>Wearing apparel; furs (18)</t>
+  </si>
+  <si>
+    <t>Leather and leather products (19)</t>
+  </si>
+  <si>
+    <t>Wood and products of wood and cork (except furniture); articles of straw and plaiting materials (20)</t>
+  </si>
+  <si>
+    <t>Printed matter and recorded media (22)</t>
+  </si>
+  <si>
+    <t>Rubber and plastic products (25)</t>
+  </si>
+  <si>
+    <t>Fabricated metal products, except machinery and equipment (28)</t>
+  </si>
+  <si>
+    <t>Machinery and equipment n.e.c. (29)</t>
+  </si>
+  <si>
+    <t>Office machinery and computers (30)</t>
+  </si>
+  <si>
+    <t>Electrical machinery and apparatus n.e.c. (31)</t>
+  </si>
+  <si>
+    <t>Radio, television and communication equipment and apparatus (32)</t>
+  </si>
+  <si>
+    <t>Medical, precision and optical instruments, watches and clocks (33)</t>
+  </si>
+  <si>
+    <t>Motor vehicles, trailers and semi-trailers (34)</t>
+  </si>
+  <si>
+    <t>Other transport equipment (35)</t>
+  </si>
+  <si>
+    <t>Furniture; other manufactured goods n.e.c. (36)</t>
+  </si>
+  <si>
+    <t>Collected and purified water, distribution services of water (41)</t>
+  </si>
+  <si>
+    <t>Construction work (45)</t>
+  </si>
+  <si>
+    <t>Wholesale trade and commission trade services, except of motor vehicles and motorcycles (51)</t>
+  </si>
+  <si>
+    <t>Retail  trade services, except of motor vehicles and motorcycles; repair services of personal and household goods (52)</t>
+  </si>
+  <si>
+    <t>Hotel and restaurant services (55)</t>
+  </si>
+  <si>
+    <t>Air transport services (62)</t>
+  </si>
+  <si>
+    <t>Supporting and auxiliary transport services; travel agency services (63)</t>
+  </si>
+  <si>
+    <t>Post and telecommunication services (64)</t>
+  </si>
+  <si>
+    <t>Financial intermediation services, except insurance and pension funding services (65)</t>
+  </si>
+  <si>
+    <t>Insurance and pension funding services, except compulsory social security services (66)</t>
+  </si>
+  <si>
+    <t>Services auxiliary to financial intermediation (67)</t>
+  </si>
+  <si>
+    <t>Real estate services (70)</t>
+  </si>
+  <si>
+    <t>Renting services of machinery and equipment without operator and of personal and household goods (71)</t>
+  </si>
+  <si>
+    <t>Computer and related services (72)</t>
+  </si>
+  <si>
+    <t>Research and development services (73)</t>
+  </si>
+  <si>
+    <t>Other business services (74)</t>
+  </si>
+  <si>
+    <t>Public administration and defence services; compulsory social security services (75)</t>
+  </si>
+  <si>
+    <t>Education services (80)</t>
+  </si>
+  <si>
+    <t>Health and social work services (85)</t>
+  </si>
+  <si>
+    <t>Membership organisation services n.e.c. (91)</t>
+  </si>
+  <si>
+    <t>Recreational, cultural and sporting services (92)</t>
+  </si>
+  <si>
+    <t>Other services (93)</t>
+  </si>
+  <si>
+    <t>Private households with employed persons (95)</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1796,7 +1799,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1808,7 +1810,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2169,13 +2170,13 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1:DV1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85.28515625" customWidth="1"/>
-    <col min="2" max="126" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="85.33203125" customWidth="1"/>
+    <col min="2" max="126" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:126" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:126" s="2" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
         <v>163</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2600,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2624,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2648,7 +2649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2656,7 +2657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2672,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2680,7 +2681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2721,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2745,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2761,7 +2762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2825,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2833,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2841,7 +2842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2881,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2889,7 +2890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2897,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2905,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2921,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -2929,7 +2930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -2937,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2945,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2953,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -2991,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -2999,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -3010,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -3075,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -3165,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -3173,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -3200,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -3216,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -3224,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -3240,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -3248,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -3272,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -3296,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -3304,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -3312,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -3320,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -3347,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -3355,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -3382,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -3390,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -3425,7 +3426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -3433,7 +3434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -3441,7 +3442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -3449,7 +3450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -3465,7 +3466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -3473,7 +3474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -3495,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -3511,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
@@ -3522,7 +3523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:124" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:124" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -3585,7 +3586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -3593,7 +3594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -3601,7 +3602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -3609,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -3617,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -3628,7 +3629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
@@ -3636,7 +3637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -3666,7 +3667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -3682,7 +3683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
@@ -3690,7 +3691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -3712,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
@@ -3720,7 +3721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -3728,7 +3729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
@@ -3747,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
@@ -3766,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
@@ -3774,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -3824,7 +3825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -3848,7 +3849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -3856,7 +3857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -3864,7 +3865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -3872,7 +3873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -3880,7 +3881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
@@ -3896,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
@@ -3904,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
@@ -3920,7 +3921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
@@ -3928,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -3936,7 +3937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -3960,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -3968,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -3984,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:126" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -4006,7 +4007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -4014,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -4022,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:70" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -4045,288 +4046,288 @@
   <dimension ref="A1:CO204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B194" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CO33" sqref="CO33"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" ht="141.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:93" ht="142" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AI1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AK1" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AL1" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AM1" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AN1" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AO1" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AP1" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AR1" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AS1" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="AT1" s="9" t="s">
+      <c r="AT1" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AU1" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="AV1" s="9" t="s">
+      <c r="AV1" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="AW1" s="9" t="s">
+      <c r="AW1" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="AX1" s="9" t="s">
+      <c r="AX1" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="AY1" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ1" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BA1" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BB1" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="BC1" s="9" t="s">
+      <c r="BC1" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="BD1" s="9" t="s">
+      <c r="BD1" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="BE1" s="9" t="s">
+      <c r="BE1" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BF1" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="BG1" s="9" t="s">
+      <c r="BG1" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="BH1" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BI1" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="BJ1" s="9" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BK1" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BL1" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="BM1" s="9" t="s">
+      <c r="BM1" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="BN1" s="9" t="s">
+      <c r="BN1" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="BO1" s="9" t="s">
+      <c r="BO1" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="BP1" s="9" t="s">
+      <c r="BP1" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="BQ1" s="9" t="s">
+      <c r="BQ1" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="BR1" s="9" t="s">
+      <c r="BR1" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="BS1" s="7" t="s">
+      <c r="BS1" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="BT1" s="7" t="s">
+      <c r="BT1" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="BU1" s="7" t="s">
+      <c r="BU1" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="BV1" s="7" t="s">
+      <c r="BV1" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="BW1" s="7" t="s">
+      <c r="BW1" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="BX1" s="7" t="s">
+      <c r="BX1" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="BY1" s="7" t="s">
+      <c r="BY1" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="BZ1" s="7" t="s">
+      <c r="BZ1" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="CA1" s="7" t="s">
+      <c r="CA1" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="CB1" s="7" t="s">
+      <c r="CB1" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="CC1" s="7" t="s">
+      <c r="CC1" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="CD1" s="7" t="s">
+      <c r="CD1" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="CE1" s="7" t="s">
+      <c r="CE1" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="CF1" s="7" t="s">
+      <c r="CF1" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="CG1" s="7" t="s">
+      <c r="CG1" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="CH1" s="7" t="s">
+      <c r="CH1" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="CI1" s="7" t="s">
+      <c r="CI1" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="CJ1" s="7" t="s">
+      <c r="CJ1" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="CK1" s="7" t="s">
+      <c r="CK1" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="CL1" s="8" t="s">
+      <c r="CL1" s="7" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>372</v>
       </c>
       <c r="B2">
@@ -4604,8 +4605,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>373</v>
       </c>
       <c r="B3">
@@ -4883,8 +4884,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>374</v>
       </c>
       <c r="B4">
@@ -5162,8 +5163,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>375</v>
       </c>
       <c r="B5">
@@ -5441,8 +5442,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>376</v>
       </c>
       <c r="B6">
@@ -5720,8 +5721,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>377</v>
       </c>
       <c r="B7">
@@ -5999,8 +6000,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>378</v>
       </c>
       <c r="B8">
@@ -6278,8 +6279,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>379</v>
       </c>
       <c r="B9">
@@ -6557,8 +6558,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>380</v>
       </c>
       <c r="B10">
@@ -6836,8 +6837,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>381</v>
       </c>
       <c r="B11">
@@ -7115,8 +7116,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>382</v>
       </c>
       <c r="B12">
@@ -7394,8 +7395,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -7673,8 +7674,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
@@ -7952,8 +7953,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -8231,8 +8232,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+    <row r="16" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -8510,8 +8511,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>383</v>
       </c>
       <c r="B17">
@@ -8789,8 +8790,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>384</v>
       </c>
       <c r="B18">
@@ -9068,9 +9069,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>385</v>
+    <row r="19" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>518</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -9347,9 +9348,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>386</v>
+    <row r="20" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>519</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -9626,9 +9627,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>387</v>
+    <row r="21" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>385</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -9905,9 +9906,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>388</v>
+    <row r="22" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>386</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -10184,9 +10185,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>389</v>
+    <row r="23" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>387</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -10463,9 +10464,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>390</v>
+    <row r="24" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>388</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -10742,9 +10743,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>391</v>
+    <row r="25" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>389</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -11021,9 +11022,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>392</v>
+    <row r="26" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>390</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11300,9 +11301,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>393</v>
+    <row r="27" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>391</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11579,9 +11580,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>394</v>
+    <row r="28" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>392</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -11858,9 +11859,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>395</v>
+    <row r="29" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>393</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -12137,9 +12138,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>396</v>
+    <row r="30" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>394</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -12416,9 +12417,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>397</v>
+    <row r="31" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>395</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -12695,9 +12696,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>398</v>
+    <row r="32" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>396</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -12974,9 +12975,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>399</v>
+    <row r="33" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>520</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -13253,9 +13254,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>400</v>
+    <row r="34" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>397</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -13532,9 +13533,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>401</v>
+    <row r="35" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>398</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -13811,9 +13812,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>402</v>
+    <row r="36" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>399</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -14090,9 +14091,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>403</v>
+    <row r="37" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>400</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -14369,9 +14370,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>404</v>
+    <row r="38" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>401</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -14648,9 +14649,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>405</v>
+    <row r="39" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>402</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -14927,9 +14928,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>406</v>
+    <row r="40" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>403</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -15206,9 +15207,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>407</v>
+    <row r="41" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>404</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -15485,9 +15486,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>408</v>
+    <row r="42" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>405</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -15764,9 +15765,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>409</v>
+    <row r="43" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>406</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -16043,9 +16044,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>410</v>
+    <row r="44" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>407</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -16322,9 +16323,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>411</v>
+    <row r="45" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>408</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -16601,9 +16602,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>412</v>
+    <row r="46" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>409</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -16880,9 +16881,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>413</v>
+    <row r="47" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>410</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -17159,9 +17160,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>414</v>
+    <row r="48" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>411</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -17438,9 +17439,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>415</v>
+    <row r="49" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>412</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -17717,8 +17718,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="50" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>40</v>
       </c>
       <c r="B50">
@@ -17996,9 +17997,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>416</v>
+    <row r="51" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>413</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -18275,9 +18276,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>417</v>
+    <row r="52" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>414</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -18554,9 +18555,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>418</v>
+    <row r="53" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>415</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -18833,9 +18834,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>419</v>
+    <row r="54" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>416</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -19112,9 +19113,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>420</v>
+    <row r="55" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>521</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -19391,9 +19392,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>421</v>
+    <row r="56" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>522</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -19670,9 +19671,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>422</v>
+    <row r="57" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>523</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -19949,9 +19950,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>423</v>
+    <row r="58" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>524</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -20228,9 +20229,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
-        <v>424</v>
+    <row r="59" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>525</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -20507,9 +20508,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>425</v>
+    <row r="60" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>417</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -20786,8 +20787,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="61" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>51</v>
       </c>
       <c r="B61">
@@ -21065,9 +21066,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>426</v>
+    <row r="62" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>418</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -21344,9 +21345,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>427</v>
+    <row r="63" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>419</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -21623,9 +21624,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>428</v>
+    <row r="64" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>526</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -21902,9 +21903,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>429</v>
+    <row r="65" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>420</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -22181,9 +22182,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>430</v>
+    <row r="66" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>421</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -22460,9 +22461,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>431</v>
+    <row r="67" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>422</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -22739,9 +22740,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>432</v>
+    <row r="68" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>423</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -23018,9 +23019,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>433</v>
+    <row r="69" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>424</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -23297,9 +23298,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>434</v>
+    <row r="70" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>425</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -23576,9 +23577,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>435</v>
+    <row r="71" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>426</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -23855,9 +23856,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>436</v>
+    <row r="72" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>427</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -24134,9 +24135,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>437</v>
+    <row r="73" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>428</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -24413,9 +24414,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>438</v>
+    <row r="74" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>429</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -24692,9 +24693,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>439</v>
+    <row r="75" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>430</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -24971,9 +24972,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>440</v>
+    <row r="76" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>431</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -25250,9 +25251,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>441</v>
+    <row r="77" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>432</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -25529,9 +25530,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>442</v>
+    <row r="78" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>433</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -25808,9 +25809,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>443</v>
+    <row r="79" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>434</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -26087,9 +26088,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>444</v>
+    <row r="80" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>435</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -26366,9 +26367,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>445</v>
+    <row r="81" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>436</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -26645,9 +26646,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>446</v>
+    <row r="82" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>437</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -26924,9 +26925,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>447</v>
+    <row r="83" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>438</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -27203,9 +27204,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>448</v>
+    <row r="84" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>439</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -27482,9 +27483,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>449</v>
+    <row r="85" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>440</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -27761,9 +27762,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>450</v>
+    <row r="86" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>441</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -28040,8 +28041,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="87" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>58</v>
       </c>
       <c r="B87">
@@ -28319,9 +28320,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>451</v>
+    <row r="88" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>442</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -28598,8 +28599,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="89" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>60</v>
       </c>
       <c r="B89">
@@ -28877,8 +28878,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+    <row r="90" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>61</v>
       </c>
       <c r="B90">
@@ -29156,8 +29157,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="91" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>62</v>
       </c>
       <c r="B91">
@@ -29435,9 +29436,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>452</v>
+    <row r="92" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>443</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -29714,9 +29715,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>453</v>
+    <row r="93" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>444</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -29993,9 +29994,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>454</v>
+    <row r="94" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>445</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -30272,9 +30273,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>455</v>
+    <row r="95" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>446</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -30551,9 +30552,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>456</v>
+    <row r="96" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>447</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -30830,9 +30831,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>457</v>
+    <row r="97" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>527</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -31109,9 +31110,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>458</v>
+    <row r="98" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>448</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -31388,9 +31389,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>459</v>
+    <row r="99" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>449</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -31667,9 +31668,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>460</v>
+    <row r="100" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>450</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -31946,9 +31947,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>461</v>
+    <row r="101" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>451</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -32225,9 +32226,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>462</v>
+    <row r="102" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>452</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -32504,9 +32505,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>463</v>
+    <row r="103" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>453</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -32783,9 +32784,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>464</v>
+    <row r="104" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>454</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -33062,9 +33063,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>465</v>
+    <row r="105" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>455</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -33341,9 +33342,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>466</v>
+    <row r="106" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>456</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -33620,9 +33621,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>467</v>
+    <row r="107" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>457</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -33899,9 +33900,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>468</v>
+    <row r="108" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>458</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -34178,9 +34179,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>469</v>
+    <row r="109" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>459</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -34457,9 +34458,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>470</v>
+    <row r="110" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>460</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -34736,9 +34737,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>471</v>
+    <row r="111" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>461</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -35015,9 +35016,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>472</v>
+    <row r="112" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>462</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -35294,9 +35295,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>473</v>
+    <row r="113" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>463</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -35573,9 +35574,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>474</v>
+    <row r="114" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>464</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -35852,9 +35853,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>475</v>
+    <row r="115" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>465</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -36131,9 +36132,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>476</v>
+    <row r="116" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>466</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -36410,9 +36411,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>477</v>
+    <row r="117" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>467</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -36689,9 +36690,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>478</v>
+    <row r="118" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>528</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -36968,9 +36969,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>479</v>
+    <row r="119" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>529</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -37247,9 +37248,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>480</v>
+    <row r="120" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>530</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -37526,9 +37527,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>481</v>
+    <row r="121" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>531</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -37805,9 +37806,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>482</v>
+    <row r="122" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>532</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -38084,9 +38085,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>483</v>
+    <row r="123" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>533</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -38363,9 +38364,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>484</v>
+    <row r="124" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>534</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -38642,9 +38643,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>485</v>
+    <row r="125" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>535</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -38921,9 +38922,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>486</v>
+    <row r="126" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>536</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -39200,9 +39201,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>487</v>
+    <row r="127" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>468</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -39479,9 +39480,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>488</v>
+    <row r="128" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>469</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -39758,9 +39759,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>489</v>
+    <row r="129" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>470</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -40037,9 +40038,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
-        <v>490</v>
+    <row r="130" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>471</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -40316,9 +40317,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>491</v>
+    <row r="131" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>472</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -40595,9 +40596,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>492</v>
+    <row r="132" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>473</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -40874,9 +40875,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>493</v>
+    <row r="133" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>474</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -41153,9 +41154,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>494</v>
+    <row r="134" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>475</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -41432,9 +41433,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>495</v>
+    <row r="135" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>476</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -41711,9 +41712,9 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="136" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>496</v>
+    <row r="136" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>477</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -41990,9 +41991,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
-        <v>497</v>
+    <row r="137" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>478</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -42269,9 +42270,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
-        <v>498</v>
+    <row r="138" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>479</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -42548,9 +42549,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
-        <v>499</v>
+    <row r="139" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>480</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -42827,9 +42828,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
-        <v>500</v>
+    <row r="140" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>481</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -43106,9 +43107,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
-        <v>501</v>
+    <row r="141" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>482</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -43385,9 +43386,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
-        <v>502</v>
+    <row r="142" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>483</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -43664,9 +43665,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>503</v>
+    <row r="143" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>484</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -43943,9 +43944,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>504</v>
+    <row r="144" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>485</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -44222,9 +44223,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>505</v>
+    <row r="145" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>486</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -44501,9 +44502,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
-        <v>506</v>
+    <row r="146" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>487</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -44780,9 +44781,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>507</v>
+    <row r="147" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>488</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -45059,9 +45060,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>508</v>
+    <row r="148" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>489</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -45338,9 +45339,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>509</v>
+    <row r="149" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>490</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -45617,9 +45618,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>510</v>
+    <row r="150" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>537</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -45693,10 +45694,10 @@
       <c r="Y150">
         <v>0</v>
       </c>
-      <c r="Z150" s="6">
+      <c r="Z150" s="5">
         <v>0.5</v>
       </c>
-      <c r="AA150" s="6">
+      <c r="AA150" s="5">
         <v>0.5</v>
       </c>
       <c r="AB150">
@@ -45896,9 +45897,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>511</v>
+    <row r="151" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>538</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -46175,9 +46176,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>512</v>
+    <row r="152" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>491</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -46454,8 +46455,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
+    <row r="153" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>114</v>
       </c>
       <c r="B153">
@@ -46733,9 +46734,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
-        <v>513</v>
+    <row r="154" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>492</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -47012,9 +47013,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
-        <v>514</v>
+    <row r="155" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>539</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -47291,9 +47292,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>515</v>
+    <row r="156" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>540</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -47570,9 +47571,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
-        <v>516</v>
+    <row r="157" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>541</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -47849,9 +47850,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
-        <v>517</v>
+    <row r="158" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>493</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -48128,9 +48129,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>518</v>
+    <row r="159" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>494</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -48407,9 +48408,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
-        <v>519</v>
+    <row r="160" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>495</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -48686,9 +48687,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
-        <v>520</v>
+    <row r="161" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>496</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -48965,9 +48966,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>521</v>
+    <row r="162" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>497</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -49244,9 +49245,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
-        <v>522</v>
+    <row r="163" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>542</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -49523,9 +49524,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
-        <v>523</v>
+    <row r="164" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>543</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -49802,9 +49803,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
-        <v>524</v>
+    <row r="165" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>544</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -50081,9 +50082,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>525</v>
+    <row r="166" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>545</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -50360,9 +50361,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>526</v>
+    <row r="167" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>546</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -50639,9 +50640,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
-        <v>527</v>
+    <row r="168" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>547</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -50918,9 +50919,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>528</v>
+    <row r="169" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>548</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -51197,9 +51198,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A170" s="11" t="s">
-        <v>529</v>
+    <row r="170" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>549</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -51476,9 +51477,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A171" s="11" t="s">
-        <v>530</v>
+    <row r="171" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>550</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -51755,9 +51756,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A172" s="11" t="s">
-        <v>531</v>
+    <row r="172" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>551</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -52034,9 +52035,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A173" s="11" t="s">
-        <v>532</v>
+    <row r="173" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>552</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -52161,10 +52162,10 @@
       <c r="AP173">
         <v>0</v>
       </c>
-      <c r="AQ173" s="10">
+      <c r="AQ173" s="9">
         <v>0.11111111111111108</v>
       </c>
-      <c r="AR173" s="10">
+      <c r="AR173" s="9">
         <v>0.11111111111111108</v>
       </c>
       <c r="AS173">
@@ -52185,31 +52186,31 @@
       <c r="AX173">
         <v>0</v>
       </c>
-      <c r="AY173" s="10">
+      <c r="AY173" s="9">
         <v>0.11111111111111108</v>
       </c>
-      <c r="AZ173" s="10">
+      <c r="AZ173" s="9">
         <v>0.11111111111111108</v>
       </c>
       <c r="BA173">
         <v>0</v>
       </c>
-      <c r="BB173" s="10">
+      <c r="BB173" s="9">
         <v>0.11111111111111108</v>
       </c>
-      <c r="BC173" s="10">
+      <c r="BC173" s="9">
         <v>0.11111111111111108</v>
       </c>
       <c r="BD173">
         <v>0</v>
       </c>
-      <c r="BE173" s="10">
+      <c r="BE173" s="9">
         <v>0.11111111111111108</v>
       </c>
-      <c r="BF173" s="10">
+      <c r="BF173" s="9">
         <v>0.11111111111111108</v>
       </c>
-      <c r="BG173" s="10">
+      <c r="BG173" s="9">
         <v>0.11111111111111108</v>
       </c>
       <c r="BH173">
@@ -52313,9 +52314,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A174" s="11" t="s">
-        <v>533</v>
+    <row r="174" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>553</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -52592,9 +52593,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A175" s="11" t="s">
-        <v>534</v>
+    <row r="175" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>554</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -52871,9 +52872,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A176" s="11" t="s">
-        <v>535</v>
+    <row r="176" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>555</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -53150,9 +53151,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A177" s="11" t="s">
-        <v>536</v>
+    <row r="177" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>498</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -53429,9 +53430,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A178" s="11" t="s">
-        <v>537</v>
+    <row r="178" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>499</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -53708,9 +53709,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A179" s="11" t="s">
-        <v>538</v>
+    <row r="179" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>500</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -53987,9 +53988,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A180" s="11" t="s">
-        <v>539</v>
+    <row r="180" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>501</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -54266,9 +54267,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A181" s="11" t="s">
-        <v>540</v>
+    <row r="181" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>502</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -54545,9 +54546,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A182" s="11" t="s">
-        <v>541</v>
+    <row r="182" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>503</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -54824,9 +54825,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A183" s="11" t="s">
-        <v>542</v>
+    <row r="183" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>504</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -55103,9 +55104,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A184" s="11" t="s">
-        <v>543</v>
+    <row r="184" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>505</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -55382,9 +55383,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A185" s="11" t="s">
-        <v>544</v>
+    <row r="185" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>506</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -55661,9 +55662,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A186" s="11" t="s">
-        <v>545</v>
+    <row r="186" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>507</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -55940,9 +55941,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A187" s="11" t="s">
-        <v>546</v>
+    <row r="187" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>508</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -56219,9 +56220,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A188" s="11" t="s">
-        <v>547</v>
+    <row r="188" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>509</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -56498,9 +56499,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A189" s="11" t="s">
-        <v>548</v>
+    <row r="189" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>510</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -56777,9 +56778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A190" s="11" t="s">
-        <v>549</v>
+    <row r="190" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>511</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -57056,9 +57057,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A191" s="11" t="s">
-        <v>550</v>
+    <row r="191" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>512</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -57335,9 +57336,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A192" s="11" t="s">
-        <v>551</v>
+    <row r="192" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>513</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -57614,9 +57615,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A193" s="11" t="s">
-        <v>552</v>
+    <row r="193" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>514</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -57893,9 +57894,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A194" s="11" t="s">
-        <v>553</v>
+    <row r="194" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>515</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -58172,9 +58173,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A195" s="11" t="s">
-        <v>554</v>
+    <row r="195" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>516</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -58451,9 +58452,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A196" s="11" t="s">
-        <v>555</v>
+    <row r="196" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>517</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -58730,8 +58731,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A197" s="11" t="s">
+    <row r="197" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
         <v>556</v>
       </c>
       <c r="B197">
@@ -59009,8 +59010,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A198" s="11" t="s">
+    <row r="198" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
         <v>557</v>
       </c>
       <c r="B198">
@@ -59288,8 +59289,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A199" s="11" t="s">
+    <row r="199" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
         <v>558</v>
       </c>
       <c r="B199">
@@ -59567,9 +59568,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A200" s="11" t="s">
-        <v>161</v>
+    <row r="200" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>559</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -59846,8 +59847,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A201" s="11" t="s">
+    <row r="201" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
         <v>162</v>
       </c>
       <c r="B201">
@@ -60125,13 +60126,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A202" s="12"/>
+    <row r="202" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A202" s="10"/>
     </row>
-    <row r="203" spans="1:93" x14ac:dyDescent="0.25">
-      <c r="A203" s="12"/>
+    <row r="203" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="A203" s="10"/>
     </row>
-    <row r="204" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:93" x14ac:dyDescent="0.2">
       <c r="B204">
         <f t="shared" ref="B204:BN204" si="4">SUM(B2:B201)</f>
         <v>17</v>

</xml_diff>